<commit_message>
test questions as nodes
</commit_message>
<xml_diff>
--- a/assets/excels/2024_IEO_econ_MCQ_PersonalScores.xlsx
+++ b/assets/excels/2024_IEO_econ_MCQ_PersonalScores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigohernandez/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76B2CBD2-7177-4D4A-8B59-BBFEC01AC177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE03664C-EBF9-7741-BF56-3470FCACFD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3669C2C9-FAB8-644D-91AF-BEEA05D341B0}"/>
   </bookViews>
@@ -113,18 +113,12 @@
     <t>Opportunity cost, competitive advantage</t>
   </si>
   <si>
-    <t>Firm’s behavior</t>
-  </si>
-  <si>
     <t>Non-competitive markets</t>
   </si>
   <si>
     <t>Game theory</t>
   </si>
   <si>
-    <t>Consumer’s choice</t>
-  </si>
-  <si>
     <t>Consumer surplus, equilibrium</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t>Monetary and fiscal policy</t>
   </si>
   <si>
-    <t>Explanation and connection to examples</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nobel explanation </t>
   </si>
   <si>
@@ -183,13 +174,22 @@
   </si>
   <si>
     <t>Institutions and Inequality</t>
+  </si>
+  <si>
+    <t>Nobel research (connectivity)</t>
+  </si>
+  <si>
+    <t>Firm's behavior</t>
+  </si>
+  <si>
+    <t>Consumer's choice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +200,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -224,12 +230,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,7 +574,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
@@ -620,7 +627,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>22</v>
@@ -637,7 +644,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>24</v>
@@ -654,10 +661,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -671,10 +678,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -688,10 +695,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -705,10 +712,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -722,10 +729,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -739,10 +746,10 @@
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -756,10 +763,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -773,10 +780,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -790,10 +797,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -807,10 +814,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -824,10 +831,10 @@
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -841,10 +848,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -858,10 +865,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -874,11 +881,11 @@
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>45</v>
+      <c r="C18" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -892,10 +899,10 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -909,10 +916,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -926,10 +933,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="E21">
         <v>1</v>

</xml_diff>